<commit_message>
FSL preprocessing for triamese
</commit_message>
<xml_diff>
--- a/CSVs/OASIS3_testingData_HCCT.xlsx
+++ b/CSVs/OASIS3_testingData_HCCT.xlsx
@@ -453,33 +453,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sub-OAS30001_ses-d0129_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30001_ses-d0129_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>65</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sub-OAS30002_ses-d0371_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30002_ses-d0371_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>68</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sub-OAS30003_ses-d0558_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30003_ses-d0558_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -492,7 +492,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>sub-OAS30004_ses-d1101_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30004_ses-d1101_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -505,33 +505,33 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>sub-OAS30005_ses-d0143_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30005_ses-d0143_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>48</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sub-OAS30006_ses-d0166_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30006_ses-d0166_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>62</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>sub-OAS30008_ses-d0061_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30008_ses-d0061_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -544,7 +544,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sub-OAS30009_ses-d0148_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30009_ses-d0148_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -557,7 +557,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>sub-OAS30010_ses-d0068_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30010_ses-d0068_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -570,7 +570,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>sub-OAS30011_ses-d0055_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30011_ses-d0055_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -583,20 +583,20 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>sub-OAS30014_ses-d0196_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30014_ses-d0196_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>70</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>sub-OAS30015_ses-d0116_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30015_ses-d0116_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -609,20 +609,20 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>sub-OAS30017_ses-d0054_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30017_ses-d0054_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>53</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>sub-OAS30018_ses-d0070_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30018_ses-d0070_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>sub-OAS30020_ses-d0092_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30020_ses-d0092_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -648,20 +648,20 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>sub-OAS30021_ses-d0071_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30021_ses-d0071_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>69</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>sub-OAS30026_ses-d0048_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30026_ses-d0048_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -674,59 +674,59 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>sub-OAS30030_ses-d0170_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30030_ses-d0170_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>66</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>sub-OAS30032_ses-d0262_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30032_ses-d0262_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>50</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>sub-OAS30033_ses-d0133_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30033_ses-d0133_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>79</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>sub-OAS30034_ses-d0044_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30034_ses-d0044_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>65</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>sub-OAS30036_ses-d0059_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30036_ses-d0059_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -739,7 +739,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>sub-OAS30037_ses-d0154_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30037_ses-d0154_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -752,7 +752,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>sub-OAS30039_ses-d0103_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30039_ses-d0103_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -765,7 +765,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>sub-OAS30042_ses-d0067_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30042_ses-d0067_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -778,33 +778,33 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>sub-OAS30044_ses-d0054_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30044_ses-d0054_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>63</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>sub-OAS30046_ses-d0072_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30046_ses-d0072_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>80</v>
       </c>
       <c r="C28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>sub-OAS30048_ses-d0983_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30048_ses-d0983_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -817,33 +817,33 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>sub-OAS30049_ses-d0013_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30049_ses-d0013_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>73</v>
       </c>
       <c r="C30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>sub-OAS30050_ses-d0110_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30050_ses-d0110_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>70</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>sub-OAS30053_ses-d0428_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30053_ses-d0428_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -856,7 +856,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>sub-OAS30059_ses-d0230_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30059_ses-d0230_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -869,7 +869,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>sub-OAS30060_ses-d0074_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30060_ses-d0074_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -882,20 +882,20 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>sub-OAS30062_ses-d0087_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30062_ses-d0087_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>51</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>sub-OAS30065_ses-d0548_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30065_ses-d0548_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -908,7 +908,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>sub-OAS30066_ses-d0524_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30066_ses-d0524_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -921,7 +921,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>sub-OAS30067_ses-d0057_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30067_ses-d0057_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -934,7 +934,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>sub-OAS30073_ses-d0033_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30073_ses-d0033_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -947,20 +947,20 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>sub-OAS30075_ses-d0143_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30075_ses-d0143_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>80</v>
       </c>
       <c r="C40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>sub-OAS30077_ses-d0944_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30077_ses-d0944_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -973,20 +973,20 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>sub-OAS30079_ses-d0019_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30079_ses-d0019_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>45</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>sub-OAS30080_ses-d0048_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30080_ses-d0048_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -999,20 +999,20 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>sub-OAS30082_ses-d1700_run-02_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30082_ses-d1700_run-02_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>61</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>sub-OAS30083_ses-d0465_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30083_ses-d0465_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -1025,7 +1025,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>sub-OAS30086_ses-d0000_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30086_ses-d0000_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1038,20 +1038,20 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>sub-OAS30088_ses-d0093_run-01_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30088_ses-d0093_run-01_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>76</v>
       </c>
       <c r="C47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sub-OAS30089_ses-d0001_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30089_ses-d0001_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -1064,33 +1064,33 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sub-OAS30090_ses-d0118_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30090_ses-d0118_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>53</v>
       </c>
       <c r="C49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sub-OAS30092_ses-d0636_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30092_ses-d0636_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>60</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>sub-OAS30093_ses-d0056_T1w_Warped.nii.gz</t>
+          <t>sub-OAS30093_ses-d0056_T1w.nii.gz</t>
         </is>
       </c>
       <c r="B51" t="n">

</xml_diff>